<commit_message>
adding the sudan data plus cleaning code and dictionnary
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAL\projects\solutions-measure\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F5122E-2AA1-4F75-B57F-4A1BFF73D43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC8B39D-4880-4B1C-8638-3D2F2DB4DCF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
     <sheet name="nigeria" sheetId="1" r:id="rId2"/>
+    <sheet name="sudan" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
   <si>
     <t>indicator</t>
   </si>
@@ -286,6 +287,75 @@
   </si>
   <si>
     <t>Legally own dwelling</t>
+  </si>
+  <si>
+    <t>I1_sec_day</t>
+  </si>
+  <si>
+    <t>I3_no_borrow</t>
+  </si>
+  <si>
+    <t>I5_med_satis</t>
+  </si>
+  <si>
+    <t>I7_job_unemploy</t>
+  </si>
+  <si>
+    <t>I8_econ_account</t>
+  </si>
+  <si>
+    <t>I8_poor190</t>
+  </si>
+  <si>
+    <t>I8_poor32</t>
+  </si>
+  <si>
+    <t>I9_hlp_access</t>
+  </si>
+  <si>
+    <t>I10_doc_birth</t>
+  </si>
+  <si>
+    <t>Feeling safe at day</t>
+  </si>
+  <si>
+    <t>Borrowing for food</t>
+  </si>
+  <si>
+    <t>Own house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improved water </t>
+  </si>
+  <si>
+    <t>Improved sanitation</t>
+  </si>
+  <si>
+    <t>Satisfied with health facilities</t>
+  </si>
+  <si>
+    <t>I4_hous_ownership</t>
+  </si>
+  <si>
+    <t>Ever in school</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Bank account</t>
+  </si>
+  <si>
+    <t>Below 3.2 USD Poverty Line</t>
+  </si>
+  <si>
+    <t>Access to compensation</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Birth certificate</t>
   </si>
 </sst>
 </file>
@@ -605,16 +675,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE9ECB-0748-4915-B6B3-A38894B98147}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -636,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -647,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -658,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -669,7 +741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -680,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -691,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
@@ -702,7 +774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
@@ -713,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
@@ -724,7 +796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.2999999999999998</v>
       </c>
@@ -735,7 +807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.4</v>
       </c>
@@ -746,7 +818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -757,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.4</v>
       </c>
@@ -768,7 +840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.4</v>
       </c>
@@ -779,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.2</v>
       </c>
@@ -790,7 +862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.2</v>
       </c>
@@ -801,7 +873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4.0999999999999996</v>
       </c>
@@ -812,7 +884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>4.0999999999999996</v>
       </c>
@@ -823,7 +895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5.0999999999999996</v>
       </c>
@@ -834,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5.0999999999999996</v>
       </c>
@@ -855,16 +927,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -886,7 +960,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -897,7 +971,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
@@ -908,7 +982,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.1000000000000001</v>
       </c>
@@ -919,7 +993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.1000000000000001</v>
       </c>
@@ -930,7 +1004,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.1000000000000001</v>
       </c>
@@ -941,7 +1015,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.1000000000000001</v>
       </c>
@@ -952,7 +1026,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
@@ -963,7 +1037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2000000000000002</v>
       </c>
@@ -974,7 +1048,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -985,7 +1059,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.2000000000000002</v>
       </c>
@@ -996,7 +1070,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.2000000000000002</v>
       </c>
@@ -1007,7 +1081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -1018,7 +1092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.2000000000000002</v>
       </c>
@@ -1029,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.2000000000000002</v>
       </c>
@@ -1040,7 +1114,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2.2999999999999998</v>
       </c>
@@ -1051,7 +1125,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.4</v>
       </c>
@@ -1062,7 +1136,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -1073,7 +1147,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
@@ -1084,7 +1158,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
@@ -1095,7 +1169,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -1106,7 +1180,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
@@ -1117,7 +1191,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1128,7 +1202,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4.0999999999999996</v>
       </c>
@@ -1137,6 +1211,224 @@
       </c>
       <c r="C25" t="s">
         <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C77687-75D5-4D61-8B2A-76B9160F9A7C}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2.1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2.4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2.4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3.1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>3.2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3.2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3.2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo in colombia's dict
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAL\projects\solutions-measure\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1E221-D5D3-4933-B0B7-99491E708AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049942A8-38A1-4B96-B5E5-3472AADE9386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,9 +482,6 @@
     <t>Defaulting on utility bills</t>
   </si>
   <si>
-    <t>I8_writte_job_contract</t>
-  </si>
-  <si>
     <t>Possession of a written employment contract</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>Posession of identity document</t>
+  </si>
+  <si>
+    <t>I8_written_job_contract</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7555CF09-C5CA-4022-B3FB-2751E81DD7D3}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1843,10 +1845,10 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>148</v>
-      </c>
-      <c r="C23" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1854,10 +1856,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
         <v>150</v>
-      </c>
-      <c r="C24" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1865,10 +1867,10 @@
         <v>3.2</v>
       </c>
       <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
         <v>152</v>
-      </c>
-      <c r="C25" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,10 +1878,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
         <v>154</v>
-      </c>
-      <c r="C26" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colombia: individuals + households
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAL\projects\solutions-measure\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049942A8-38A1-4B96-B5E5-3472AADE9386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9800D13A-C507-4BFE-B78D-A6E536CE90D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
     <sheet name="nigeria" sheetId="1" r:id="rId2"/>
     <sheet name="sudan" sheetId="3" r:id="rId3"/>
-    <sheet name="colombia" sheetId="4" r:id="rId4"/>
+    <sheet name="colombia_hh" sheetId="4" r:id="rId4"/>
+    <sheet name="colombia_ind" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="156">
   <si>
     <t>indicator</t>
   </si>
@@ -1588,6 +1589,311 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7555CF09-C5CA-4022-B3FB-2751E81DD7D3}">
   <dimension ref="A1:C26"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2.4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2.4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2.4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3.1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3.1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3.2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3.2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3.2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3.2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C069BD-135B-4489-A65A-15393695ACB4}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>

</xml_diff>

<commit_message>
Final tweaks at report plus Colombia
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAL\projects\solutions-measure\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9800D13A-C507-4BFE-B78D-A6E536CE90D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93ED8BC-F7E7-489B-A9FE-4BCFB3C6124E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="169">
   <si>
     <t>indicator</t>
   </si>
@@ -505,6 +505,45 @@
   </si>
   <si>
     <t>I8_written_job_contract</t>
+  </si>
+  <si>
+    <t>Experience of security incident</t>
+  </si>
+  <si>
+    <t>I2_move</t>
+  </si>
+  <si>
+    <t>Ability to move freely</t>
+  </si>
+  <si>
+    <t>I3_meals</t>
+  </si>
+  <si>
+    <t>Above average meals per day</t>
+  </si>
+  <si>
+    <t>Written employment contract</t>
+  </si>
+  <si>
+    <t>Official educational establishment</t>
+  </si>
+  <si>
+    <t>Written tenancy agreement</t>
+  </si>
+  <si>
+    <t>Income per capita &gt; food security line</t>
+  </si>
+  <si>
+    <t>Income per capita &gt; poverty line</t>
+  </si>
+  <si>
+    <t>Natural disaster in past 12 months</t>
+  </si>
+  <si>
+    <t>Satisfaction with current income</t>
+  </si>
+  <si>
+    <t>Satisfaction with level of security</t>
   </si>
 </sst>
 </file>
@@ -822,20 +861,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE9ECB-0748-4915-B6B3-A38894B98147}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,223 +885,256 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1.2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>2.1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2.1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2.4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2.4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2.4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.4</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2.4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2.4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2.4</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>3.2</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>3.2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1080,14 +1152,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1109,7 +1181,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1120,7 +1192,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
@@ -1131,7 +1203,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.1000000000000001</v>
       </c>
@@ -1142,7 +1214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.1000000000000001</v>
       </c>
@@ -1153,7 +1225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.1000000000000001</v>
       </c>
@@ -1164,7 +1236,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.1000000000000001</v>
       </c>
@@ -1175,7 +1247,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
@@ -1186,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2000000000000002</v>
       </c>
@@ -1197,7 +1269,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -1208,7 +1280,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.2000000000000002</v>
       </c>
@@ -1219,7 +1291,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.2000000000000002</v>
       </c>
@@ -1230,7 +1302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -1241,7 +1313,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.2000000000000002</v>
       </c>
@@ -1252,7 +1324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.2000000000000002</v>
       </c>
@@ -1263,7 +1335,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2.2999999999999998</v>
       </c>
@@ -1274,7 +1346,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.4</v>
       </c>
@@ -1285,7 +1357,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -1296,7 +1368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
@@ -1307,7 +1379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
@@ -1318,7 +1390,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -1329,7 +1401,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
@@ -1340,7 +1412,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1351,7 +1423,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4.0999999999999996</v>
       </c>
@@ -1375,14 +1447,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1404,7 +1476,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1415,7 +1487,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
@@ -1426,7 +1498,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -1437,7 +1509,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -1448,7 +1520,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -1459,7 +1531,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
@@ -1470,7 +1542,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2999999999999998</v>
       </c>
@@ -1481,7 +1553,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.4</v>
       </c>
@@ -1492,7 +1564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.4</v>
       </c>
@@ -1503,7 +1575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.1</v>
       </c>
@@ -1514,7 +1586,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3.2</v>
       </c>
@@ -1525,7 +1597,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.2</v>
       </c>
@@ -1536,7 +1608,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.2</v>
       </c>
@@ -1547,7 +1619,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4.0999999999999996</v>
       </c>
@@ -1558,7 +1630,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4.0999999999999996</v>
       </c>
@@ -1569,7 +1641,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5.0999999999999996</v>
       </c>
@@ -1589,17 +1661,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7555CF09-C5CA-4022-B3FB-2751E81DD7D3}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1618,10 +1690,10 @@
         <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1629,10 +1701,10 @@
         <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -1640,10 +1712,10 @@
         <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -1654,7 +1726,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -1665,7 +1737,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -1676,7 +1748,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
@@ -1687,7 +1759,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2999999999999998</v>
       </c>
@@ -1698,7 +1770,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
@@ -1709,7 +1781,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.4</v>
       </c>
@@ -1720,7 +1792,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.4</v>
       </c>
@@ -1731,7 +1803,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -1739,10 +1811,10 @@
         <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.1</v>
       </c>
@@ -1753,7 +1825,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.1</v>
       </c>
@@ -1764,7 +1836,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.1</v>
       </c>
@@ -1775,7 +1847,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.1</v>
       </c>
@@ -1786,7 +1858,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -1797,7 +1869,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.1</v>
       </c>
@@ -1808,7 +1880,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
@@ -1816,10 +1888,10 @@
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
@@ -1827,10 +1899,10 @@
         <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -1841,7 +1913,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
@@ -1849,10 +1921,10 @@
         <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1860,10 +1932,10 @@
         <v>149</v>
       </c>
       <c r="C24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3.2</v>
       </c>
@@ -1874,7 +1946,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5.0999999999999996</v>
       </c>
@@ -1894,17 +1966,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C069BD-135B-4489-A65A-15393695ACB4}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1915,7 +1987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1926,7 +1998,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1937,7 +2009,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -1948,7 +2020,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -1959,7 +2031,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -1970,7 +2042,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -1981,7 +2053,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
@@ -1992,7 +2064,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2999999999999998</v>
       </c>
@@ -2003,7 +2075,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
@@ -2014,7 +2086,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.4</v>
       </c>
@@ -2025,7 +2097,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.4</v>
       </c>
@@ -2036,7 +2108,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -2047,7 +2119,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.1</v>
       </c>
@@ -2058,7 +2130,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.1</v>
       </c>
@@ -2069,7 +2141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.1</v>
       </c>
@@ -2080,7 +2152,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.1</v>
       </c>
@@ -2091,7 +2163,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -2102,7 +2174,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.1</v>
       </c>
@@ -2113,7 +2185,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
@@ -2124,7 +2196,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
@@ -2135,7 +2207,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
@@ -2146,7 +2218,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
@@ -2157,7 +2229,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -2168,7 +2240,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3.2</v>
       </c>
@@ -2179,7 +2251,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5.0999999999999996</v>
       </c>

</xml_diff>

<commit_message>
Revisions to Hargeisa script, security of tenure
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAL\projects\dursol-simulations\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CA5DD7-C53B-47A2-88EB-284CEE170C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A7FDF-AB6C-41CF-9EDE-2DD77F3E2D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="182">
   <si>
     <t>indicator</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Child in school</t>
   </si>
   <si>
-    <t>Mobile phone</t>
-  </si>
-  <si>
     <t>Secondary school</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>I1_sec_saf</t>
   </si>
   <si>
-    <t>I1_sec_wor</t>
-  </si>
-  <si>
     <t>I3_pay_food</t>
   </si>
   <si>
@@ -143,18 +137,12 @@
     <t>I6_ever_school</t>
   </si>
   <si>
-    <t>I6_mobile_phone</t>
-  </si>
-  <si>
     <t>I6_sec_school</t>
   </si>
   <si>
     <t>I8_rent_problems</t>
   </si>
   <si>
-    <t>I8_unexpect_expense</t>
-  </si>
-  <si>
     <t>I9_hlp_doc</t>
   </si>
   <si>
@@ -485,9 +473,6 @@
     <t>Experience of security incident</t>
   </si>
   <si>
-    <t>I2_move</t>
-  </si>
-  <si>
     <t>Ability to move freely</t>
   </si>
   <si>
@@ -522,6 +507,81 @@
   </si>
   <si>
     <t>I9_hous_ownership</t>
+  </si>
+  <si>
+    <t>Identification documents</t>
+  </si>
+  <si>
+    <t>Ability to pay for food</t>
+  </si>
+  <si>
+    <t>I8_econ_market</t>
+  </si>
+  <si>
+    <t>Access to market</t>
+  </si>
+  <si>
+    <t>I9_hlp_own</t>
+  </si>
+  <si>
+    <t>Ownership over property</t>
+  </si>
+  <si>
+    <t>I1_SDG_16.1.4</t>
+  </si>
+  <si>
+    <t>I2_DS_1.4.1</t>
+  </si>
+  <si>
+    <t>I3_DS_2.1.2</t>
+  </si>
+  <si>
+    <t>I4_SDG_11.1.1</t>
+  </si>
+  <si>
+    <t>Living outside of slums</t>
+  </si>
+  <si>
+    <t>Security of tenure</t>
+  </si>
+  <si>
+    <t>I5_DS_2.1.8</t>
+  </si>
+  <si>
+    <t>Access to essential health care</t>
+  </si>
+  <si>
+    <t>I6_SDG_4.1.2</t>
+  </si>
+  <si>
+    <t>I6_curr_school</t>
+  </si>
+  <si>
+    <t>Child currently in school</t>
+  </si>
+  <si>
+    <t>I7_SDG_8.5.2</t>
+  </si>
+  <si>
+    <t>I8_assets_num</t>
+  </si>
+  <si>
+    <t>Number of assets</t>
+  </si>
+  <si>
+    <t>I8_SDG_1.2.1</t>
+  </si>
+  <si>
+    <t>Access to HLP mechanism</t>
+  </si>
+  <si>
+    <t>I9_SDG_1.4.2</t>
+  </si>
+  <si>
+    <t>I10_DS_5.1.1</t>
+  </si>
+  <si>
+    <t>Possession of birth certificate</t>
   </si>
 </sst>
 </file>
@@ -839,20 +899,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE9ECB-0748-4915-B6B3-A38894B98147}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -863,257 +923,334 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.2</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.1</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.2000000000000002</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.2999999999999998</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2.4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2.4</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2.4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2.4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3.1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3.2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3.2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>3.2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3.2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3.2</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B30" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1130,14 +1267,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1148,268 +1285,268 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2000000000000002</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.2000000000000002</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.2000000000000002</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2.2999999999999998</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.2</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1419,20 +1556,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C77687-75D5-4D61-8B2A-76B9160F9A7C}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1443,202 +1580,257 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>2.1</v>
       </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2.4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2.4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3.1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2.4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2.4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3.1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3.2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3.2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>3.2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>3.2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3.2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B22" t="s">
         <v>161</v>
       </c>
-      <c r="C16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" t="s">
-        <v>106</v>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1650,17 +1842,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7555CF09-C5CA-4022-B3FB-2751E81DD7D3}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1671,279 +1863,279 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.1</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2.4</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.4</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.1</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.1</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.1</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3.1</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.1</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.2</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.2</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3.2</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5.0999999999999996</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision of dictionnaire to include nigeria
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A7FDF-AB6C-41CF-9EDE-2DD77F3E2D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831449BF-97D0-4107-A9E2-7E455B227060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="193">
   <si>
     <t>indicator</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Report security incident</t>
   </si>
   <si>
-    <t>Feeling safe</t>
-  </si>
-  <si>
     <t>Owning/renting house</t>
   </si>
   <si>
@@ -582,6 +579,42 @@
   </si>
   <si>
     <t>Possession of birth certificate</t>
+  </si>
+  <si>
+    <t>Feeling safe at day and night</t>
+  </si>
+  <si>
+    <t>Feeling safe from violence</t>
+  </si>
+  <si>
+    <t>Food insecurity scale</t>
+  </si>
+  <si>
+    <t>I4_house_indurable</t>
+  </si>
+  <si>
+    <t>Indurable housing structure</t>
+  </si>
+  <si>
+    <t>I4_hous_permanent</t>
+  </si>
+  <si>
+    <t>Permanent housing structure</t>
+  </si>
+  <si>
+    <t>I6_edu_dist</t>
+  </si>
+  <si>
+    <t>Distance to school</t>
+  </si>
+  <si>
+    <t>I8_bank</t>
+  </si>
+  <si>
+    <t>I9_hlp_compensation</t>
+  </si>
+  <si>
+    <t>Tenure security</t>
   </si>
 </sst>
 </file>
@@ -901,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE9ECB-0748-4915-B6B3-A38894B98147}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,7 +964,7 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -950,7 +983,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -961,10 +994,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -972,7 +1005,7 @@
         <v>2.1</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -983,10 +1016,10 @@
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
         <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1049,10 +1082,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
         <v>166</v>
-      </c>
-      <c r="C13" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,10 +1115,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" t="s">
         <v>169</v>
-      </c>
-      <c r="C16" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1104,7 +1137,7 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1126,10 +1159,10 @@
         <v>2.4</v>
       </c>
       <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" t="s">
         <v>172</v>
-      </c>
-      <c r="C20" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1137,10 +1170,10 @@
         <v>3.1</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1159,7 +1192,7 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1170,10 +1203,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" t="s">
         <v>175</v>
-      </c>
-      <c r="C24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1181,10 +1214,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1214,10 +1247,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1225,7 +1258,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -1247,10 +1280,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1261,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,54 +1389,54 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1411,10 +1444,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1422,10 +1455,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1433,10 +1466,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1444,109 +1477,274 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>3.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2.4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2.4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2.4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>3.1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3.2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>3.2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3.2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>3.2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>3.2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3.2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3.2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B37" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
-        <v>79</v>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1585,10 +1783,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1629,10 +1827,10 @@
         <v>2.1</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1643,7 +1841,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1651,10 +1849,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1665,7 +1863,7 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1676,7 +1874,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1684,10 +1882,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1698,7 +1896,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1717,10 +1915,10 @@
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1728,10 +1926,10 @@
         <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1739,10 +1937,10 @@
         <v>3.2</v>
       </c>
       <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
         <v>159</v>
-      </c>
-      <c r="C16" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1750,10 +1948,10 @@
         <v>3.2</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1761,10 +1959,10 @@
         <v>3.2</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1772,10 +1970,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1783,10 +1981,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1797,7 +1995,7 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1805,10 +2003,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" t="s">
         <v>161</v>
-      </c>
-      <c r="C22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1816,10 +2014,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1830,7 +2028,7 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1868,10 +2066,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1879,10 +2077,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1890,10 +2088,10 @@
         <v>2.1</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1901,10 +2099,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
         <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1912,10 +2110,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1923,10 +2121,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
         <v>110</v>
-      </c>
-      <c r="C7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1934,10 +2132,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
         <v>112</v>
-      </c>
-      <c r="C8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1945,10 +2143,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
         <v>114</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1956,10 +2154,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
         <v>116</v>
-      </c>
-      <c r="C10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1967,10 +2165,10 @@
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
         <v>118</v>
-      </c>
-      <c r="C11" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1978,10 +2176,10 @@
         <v>2.4</v>
       </c>
       <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1989,10 +2187,10 @@
         <v>2.4</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2000,10 +2198,10 @@
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
         <v>123</v>
-      </c>
-      <c r="C14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2011,10 +2209,10 @@
         <v>3.1</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2022,10 +2220,10 @@
         <v>3.1</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2033,10 +2231,10 @@
         <v>3.1</v>
       </c>
       <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
         <v>129</v>
-      </c>
-      <c r="C17" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -2044,10 +2242,10 @@
         <v>3.1</v>
       </c>
       <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" t="s">
         <v>131</v>
-      </c>
-      <c r="C18" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2055,10 +2253,10 @@
         <v>3.1</v>
       </c>
       <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
         <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2069,7 +2267,7 @@
         <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2077,10 +2275,10 @@
         <v>3.2</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2088,10 +2286,10 @@
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
         <v>136</v>
-      </c>
-      <c r="C22" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2099,10 +2297,10 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2110,10 +2308,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2121,10 +2319,10 @@
         <v>3.2</v>
       </c>
       <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
         <v>139</v>
-      </c>
-      <c r="C25" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2132,10 +2330,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" t="s">
         <v>141</v>
-      </c>
-      <c r="C26" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated dict for Sudan
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831449BF-97D0-4107-A9E2-7E455B227060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA8A538-C608-4B61-838D-BC35F0B40682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="190">
   <si>
     <t>indicator</t>
   </si>
@@ -134,9 +134,6 @@
     <t>I6_educ_child</t>
   </si>
   <si>
-    <t>I6_ever_school</t>
-  </si>
-  <si>
     <t>I6_sec_school</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>I9_hlp_restored</t>
   </si>
   <si>
-    <t>I10_doc_id</t>
-  </si>
-  <si>
     <t>I10_doc_replace</t>
   </si>
   <si>
@@ -281,18 +275,12 @@
     <t>I3_no_borrow</t>
   </si>
   <si>
-    <t>I5_med_satis</t>
-  </si>
-  <si>
     <t>I7_job_unemploy</t>
   </si>
   <si>
     <t>I8_econ_account</t>
   </si>
   <si>
-    <t>I8_poor190</t>
-  </si>
-  <si>
     <t>I8_poor32</t>
   </si>
   <si>
@@ -503,12 +491,6 @@
     <t>Satisfaction with level of security</t>
   </si>
   <si>
-    <t>I9_hous_ownership</t>
-  </si>
-  <si>
-    <t>Identification documents</t>
-  </si>
-  <si>
     <t>Ability to pay for food</t>
   </si>
   <si>
@@ -615,6 +597,15 @@
   </si>
   <si>
     <t>Tenure security</t>
+  </si>
+  <si>
+    <t>Overcrowded housing</t>
+  </si>
+  <si>
+    <t>Permanent housing structures</t>
+  </si>
+  <si>
+    <t>Employed</t>
   </si>
 </sst>
 </file>
@@ -935,7 +926,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,10 +952,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -983,7 +974,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -994,10 +985,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1005,7 +996,7 @@
         <v>2.1</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1016,10 +1007,10 @@
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,10 +1073,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1115,10 +1106,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1137,7 +1128,7 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1148,7 +1139,7 @@
         <v>2.4</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -1159,10 +1150,10 @@
         <v>2.4</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1170,10 +1161,10 @@
         <v>3.1</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1181,7 +1172,7 @@
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1192,7 +1183,7 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1203,10 +1194,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1214,10 +1205,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1225,7 +1216,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -1236,7 +1227,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
@@ -1247,10 +1238,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1258,7 +1249,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -1269,7 +1260,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>21</v>
@@ -1280,10 +1271,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1296,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1323,10 +1314,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1334,10 +1325,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1345,10 +1336,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1356,10 +1347,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1367,10 +1358,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1378,10 +1369,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1389,10 +1380,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1400,10 +1391,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1414,7 +1405,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1422,10 +1413,10 @@
         <v>1.2</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1433,10 +1424,10 @@
         <v>2.1</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1444,10 +1435,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C13" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1466,10 +1457,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1477,10 +1468,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1488,10 +1479,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1499,10 +1490,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1521,10 +1512,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1543,10 +1534,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1554,10 +1545,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1565,10 +1556,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1576,10 +1567,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1587,10 +1578,10 @@
         <v>2.4</v>
       </c>
       <c r="B26" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1598,10 +1589,10 @@
         <v>2.4</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1609,10 +1600,10 @@
         <v>2.4</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1620,10 +1611,10 @@
         <v>3.1</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1631,10 +1622,10 @@
         <v>3.2</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1642,10 +1633,10 @@
         <v>3.2</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1653,10 +1644,10 @@
         <v>3.2</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1664,10 +1655,10 @@
         <v>3.2</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1675,10 +1666,10 @@
         <v>3.2</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1686,10 +1677,10 @@
         <v>3.2</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1697,10 +1688,10 @@
         <v>3.2</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1708,10 +1699,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1719,10 +1710,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1730,10 +1721,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1741,7 +1732,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
@@ -1754,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C77687-75D5-4D61-8B2A-76B9160F9A7C}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1783,10 +1774,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1794,10 +1785,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1805,10 +1796,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1816,21 +1807,21 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>2.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1838,32 +1829,32 @@
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1871,164 +1862,252 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>3.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>3.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>3.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>4.0999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>4.0999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>5.0999999999999996</v>
+        <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
+        <v>3.2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>3.2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>3.2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>156</v>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2066,10 +2145,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2077,10 +2156,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2088,10 +2167,10 @@
         <v>2.1</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2099,10 +2178,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2110,10 +2189,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2121,10 +2200,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2132,10 +2211,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2143,10 +2222,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2154,10 +2233,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2165,10 +2244,10 @@
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -2176,10 +2255,10 @@
         <v>2.4</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2187,10 +2266,10 @@
         <v>2.4</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2198,10 +2277,10 @@
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2209,10 +2288,10 @@
         <v>3.1</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2220,10 +2299,10 @@
         <v>3.1</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2231,10 +2310,10 @@
         <v>3.1</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -2242,10 +2321,10 @@
         <v>3.1</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2253,10 +2332,10 @@
         <v>3.1</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2264,10 +2343,10 @@
         <v>3.2</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2275,10 +2354,10 @@
         <v>3.2</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2286,10 +2365,10 @@
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2297,10 +2376,10 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2308,10 +2387,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2319,10 +2398,10 @@
         <v>3.2</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2330,10 +2409,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision of indicators for colombia, dict
</commit_message>
<xml_diff>
--- a/Data/dict.xlsx
+++ b/Data/dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigri\Dropbox\DurableSolutions_simulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA8A538-C608-4B61-838D-BC35F0B40682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C6D53F-CBAA-4177-B686-41BB5EACB144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hargeisa" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="178">
   <si>
     <t>indicator</t>
   </si>
@@ -197,9 +197,6 @@
     <t>I8_market_dist</t>
   </si>
   <si>
-    <t>I8_poor</t>
-  </si>
-  <si>
     <t>I8_poor125</t>
   </si>
   <si>
@@ -332,27 +329,15 @@
     <t>Birth certificate</t>
   </si>
   <si>
-    <t>I1_sec_satisfaction</t>
-  </si>
-  <si>
     <t>I1_natural_disaster</t>
   </si>
   <si>
-    <t>I3_food_secure</t>
-  </si>
-  <si>
     <t>I4_overcrowding</t>
   </si>
   <si>
     <t>Overcrowding (&gt;3 persons per room)</t>
   </si>
   <si>
-    <t>I4_legal_tenure</t>
-  </si>
-  <si>
-    <t>Legal occupancy of dwelling</t>
-  </si>
-  <si>
     <t>I4_water</t>
   </si>
   <si>
@@ -365,9 +350,6 @@
     <t>Access to improved sanitation</t>
   </si>
   <si>
-    <t>I5_health_satisfaction</t>
-  </si>
-  <si>
     <t>Satisfaction with current level of health</t>
   </si>
   <si>
@@ -383,9 +365,6 @@
     <t>Literacy</t>
   </si>
   <si>
-    <t>I6_school_attend</t>
-  </si>
-  <si>
     <t>School attendance</t>
   </si>
   <si>
@@ -401,9 +380,6 @@
     <t>I7_in_employment</t>
   </si>
   <si>
-    <t>I7_not_unemployed</t>
-  </si>
-  <si>
     <t>In employment</t>
   </si>
   <si>
@@ -438,18 +414,6 @@
   </si>
   <si>
     <t>I8_income_satisfaction</t>
-  </si>
-  <si>
-    <t>I8_child_labor</t>
-  </si>
-  <si>
-    <t>Child labor</t>
-  </si>
-  <si>
-    <t>I10_id_doc</t>
-  </si>
-  <si>
-    <t>Posession of identity document</t>
   </si>
   <si>
     <t>I8_written_job_contract</t>
@@ -955,7 +919,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -974,7 +938,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -985,10 +949,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -996,7 +960,7 @@
         <v>2.1</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1007,10 +971,10 @@
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1073,10 +1037,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1106,10 +1070,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1128,7 +1092,7 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1150,10 +1114,10 @@
         <v>2.4</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1161,10 +1125,10 @@
         <v>3.1</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1183,7 +1147,7 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1194,10 +1158,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1205,10 +1169,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1238,10 +1202,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B28" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1249,7 +1213,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -1271,10 +1235,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1287,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1281,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1328,7 +1292,7 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1339,7 +1303,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1350,7 +1314,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1361,7 +1325,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1372,7 +1336,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1380,10 +1344,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1391,10 +1355,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1405,7 +1369,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1413,10 +1377,10 @@
         <v>1.2</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1424,10 +1388,10 @@
         <v>2.1</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1435,10 +1399,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1457,10 +1421,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C15" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1471,7 +1435,7 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1482,7 +1446,7 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1493,7 +1457,7 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1515,7 +1479,7 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1537,7 +1501,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1545,10 +1509,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1559,7 +1523,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1567,10 +1531,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1578,10 +1542,10 @@
         <v>2.4</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1592,7 +1556,7 @@
         <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1600,10 +1564,10 @@
         <v>2.4</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1611,10 +1575,10 @@
         <v>3.1</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1622,10 +1586,10 @@
         <v>3.2</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1636,7 +1600,7 @@
         <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1647,7 +1611,7 @@
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1658,7 +1622,7 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1666,10 +1630,10 @@
         <v>3.2</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1677,10 +1641,10 @@
         <v>3.2</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1688,10 +1652,10 @@
         <v>3.2</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1699,10 +1663,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1710,10 +1674,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B38" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1721,10 +1685,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C39" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1732,7 +1696,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
@@ -1747,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C77687-75D5-4D61-8B2A-76B9160F9A7C}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1774,10 +1738,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1788,7 +1752,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1799,7 +1763,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1810,7 +1774,7 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1818,10 +1782,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1829,10 +1793,10 @@
         <v>2.1</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1843,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1851,10 +1815,10 @@
         <v>2.1</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1862,10 +1826,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1876,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1887,7 +1851,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1898,7 +1862,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1906,10 +1870,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1917,10 +1881,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1928,10 +1892,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1942,7 +1906,7 @@
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1950,10 +1914,10 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1961,10 +1925,10 @@
         <v>2.4</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1983,10 +1947,10 @@
         <v>3.1</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1994,10 +1958,10 @@
         <v>3.1</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2005,10 +1969,10 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2016,10 +1980,10 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2027,10 +1991,10 @@
         <v>3.2</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2038,10 +2002,10 @@
         <v>3.2</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -2049,10 +2013,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -2060,10 +2024,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2074,7 +2038,7 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -2082,10 +2046,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2093,10 +2057,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2104,7 +2068,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B32" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -2119,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7555CF09-C5CA-4022-B3FB-2751E81DD7D3}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B31" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2145,10 +2109,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2156,10 +2120,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2167,10 +2131,10 @@
         <v>2.1</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2178,10 +2142,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2189,10 +2153,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2200,10 +2164,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2211,10 +2175,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2222,10 +2186,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2233,10 +2197,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2244,10 +2208,10 @@
         <v>2.4</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -2255,10 +2219,10 @@
         <v>2.4</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2266,10 +2230,10 @@
         <v>2.4</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2277,10 +2241,10 @@
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2288,10 +2252,10 @@
         <v>3.1</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2299,10 +2263,10 @@
         <v>3.1</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2310,10 +2274,10 @@
         <v>3.1</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -2321,10 +2285,10 @@
         <v>3.1</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2332,10 +2296,10 @@
         <v>3.1</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2343,10 +2307,10 @@
         <v>3.2</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2354,10 +2318,10 @@
         <v>3.2</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2365,10 +2329,10 @@
         <v>3.2</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2376,10 +2340,10 @@
         <v>3.2</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2387,21 +2351,21 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>3.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2409,10 +2373,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>